<commit_message>
Added May 2024 Year Ends and SE extra 2024 with fixes for 2023
</commit_message>
<xml_diff>
--- a/GB Accounts 2022-23/GB Accounts SE Extra 2023-04-05 (Apr23) Excel 2007/Fixedassets050423.xlsx
+++ b/GB Accounts 2022-23/GB Accounts SE Extra 2023-04-05 (Apr23) Excel 2007/Fixedassets050423.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr showObjects="placeholders" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Downloads\Packages to create\GB Accounts SE Extra 2022-04-05 (Apr22) Excel 2007\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antony/projects/diy-accounting/GB Accounts 2022-23/GB Accounts SE Extra 2023-04-05 (Apr23) Excel 2007/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C57D9176-EC61-4C99-B0A0-9175194462C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41C8097-F8C0-B946-86ED-7545D2863FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="724" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25900" windowHeight="17440" tabRatio="724" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="11" r:id="rId1"/>
@@ -402,6 +402,7 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -423,6 +424,7 @@
       <sz val="10"/>
       <color indexed="18"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -434,6 +436,7 @@
       <sz val="10"/>
       <color indexed="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -462,6 +465,7 @@
     <font>
       <sz val="9"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -483,6 +487,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -495,6 +500,7 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1093,6 +1099,27 @@
     <xf numFmtId="9" fontId="11" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="15" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="6"/>
     </xf>
@@ -1102,14 +1129,71 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="6"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="15" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1122,96 +1206,56 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="6"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="6"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="6"/>
     </xf>
@@ -1233,43 +1277,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="6"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
@@ -1277,20 +1292,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1310,8 +1316,11 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Business Details"/>
       <sheetName val="SE Short"/>
@@ -1335,7 +1344,7 @@
       <sheetData sheetId="8">
         <row r="4">
           <cell r="B4">
-            <v>44292</v>
+            <v>44657</v>
           </cell>
           <cell r="G4">
             <v>1</v>
@@ -1376,7 +1385,7 @@
         </row>
         <row r="17">
           <cell r="B17">
-            <v>44656</v>
+            <v>45021</v>
           </cell>
           <cell r="G17">
             <v>0.25</v>
@@ -1389,22 +1398,25 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="OpeningCreditors"/>
-      <sheetName val="Apr21"/>
-      <sheetName val="May21"/>
-      <sheetName val="Jun21"/>
-      <sheetName val="Jul21"/>
-      <sheetName val="Aug21"/>
-      <sheetName val="Sep21"/>
-      <sheetName val="Oct21"/>
-      <sheetName val="Nov21"/>
-      <sheetName val="Dec21"/>
-      <sheetName val="Jan22"/>
-      <sheetName val="Feb22"/>
-      <sheetName val="Mar22"/>
+      <sheetName val="Apr22"/>
+      <sheetName val="May22"/>
+      <sheetName val="Jun22"/>
+      <sheetName val="Jul22"/>
+      <sheetName val="Aug22"/>
+      <sheetName val="Sep22"/>
+      <sheetName val="Oct22"/>
+      <sheetName val="Nov22"/>
+      <sheetName val="Dec22"/>
+      <sheetName val="Jan23"/>
+      <sheetName val="Feb23"/>
+      <sheetName val="Mar23"/>
       <sheetName val="ClosingCreditors"/>
     </sheetNames>
     <sheetDataSet>
@@ -1434,22 +1446,25 @@
 </file>
 
 <file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="OpeningDebtors"/>
-      <sheetName val="Apr21"/>
-      <sheetName val="May21"/>
-      <sheetName val="Jun21"/>
-      <sheetName val="Jul21"/>
-      <sheetName val="Aug21"/>
-      <sheetName val="Sep21"/>
-      <sheetName val="Oct21"/>
-      <sheetName val="Nov21"/>
-      <sheetName val="Dec21"/>
-      <sheetName val="Jan22"/>
-      <sheetName val="Feb22"/>
-      <sheetName val="Mar22"/>
+      <sheetName val="Apr22"/>
+      <sheetName val="May22"/>
+      <sheetName val="Jun22"/>
+      <sheetName val="Jul22"/>
+      <sheetName val="Aug22"/>
+      <sheetName val="Sep22"/>
+      <sheetName val="Oct22"/>
+      <sheetName val="Nov22"/>
+      <sheetName val="Dec22"/>
+      <sheetName val="Jan23"/>
+      <sheetName val="Feb23"/>
+      <sheetName val="Mar23"/>
       <sheetName val="ClosingDebtors"/>
     </sheetNames>
     <sheetDataSet>
@@ -1479,9 +1494,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1519,9 +1534,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1554,26 +1569,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1606,26 +1604,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1807,45 +1788,45 @@
       <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="1.7109375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="1.6640625" style="5" customWidth="1"/>
     <col min="2" max="2" width="11" style="4" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" style="80" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="31" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="9.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="23.5" style="80" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" style="31" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="11.5" style="3" customWidth="1"/>
+    <col min="8" max="8" width="6.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="9.5" style="3" customWidth="1"/>
     <col min="11" max="11" width="11" style="3" customWidth="1"/>
-    <col min="12" max="12" width="0.85546875" style="3" customWidth="1"/>
-    <col min="13" max="13" width="6.7109375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="0.85546875" style="3" customWidth="1"/>
+    <col min="12" max="12" width="0.83203125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="6.6640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="0.83203125" style="3" customWidth="1"/>
     <col min="15" max="15" width="11" style="2" customWidth="1"/>
-    <col min="16" max="16" width="5.7109375" style="89" customWidth="1"/>
-    <col min="17" max="18" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.42578125" style="2" customWidth="1"/>
-    <col min="20" max="20" width="0.85546875" style="2" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" style="4"/>
-    <col min="22" max="22" width="10.7109375" style="3" customWidth="1"/>
-    <col min="23" max="23" width="10.85546875" style="3" customWidth="1"/>
-    <col min="24" max="24" width="11.28515625" style="3" customWidth="1"/>
-    <col min="25" max="26" width="9.140625" style="2"/>
-    <col min="27" max="27" width="1.7109375" style="5" customWidth="1"/>
-    <col min="28" max="16384" width="9.140625" style="5"/>
+    <col min="16" max="16" width="5.6640625" style="89" customWidth="1"/>
+    <col min="17" max="18" width="8.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.5" style="2" customWidth="1"/>
+    <col min="20" max="20" width="0.83203125" style="2" customWidth="1"/>
+    <col min="21" max="21" width="9.1640625" style="4"/>
+    <col min="22" max="22" width="10.6640625" style="3" customWidth="1"/>
+    <col min="23" max="23" width="10.83203125" style="3" customWidth="1"/>
+    <col min="24" max="24" width="11.33203125" style="3" customWidth="1"/>
+    <col min="25" max="26" width="9.1640625" style="2"/>
+    <col min="27" max="27" width="1.6640625" style="5" customWidth="1"/>
+    <col min="28" max="16384" width="9.1640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="6" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="123"/>
-      <c r="B1" s="134" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="145" t="s">
+    <row r="1" spans="1:27" s="6" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="149"/>
+      <c r="B1" s="127" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="138" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="146"/>
+      <c r="D1" s="139"/>
       <c r="E1" s="62">
         <f>E57+E110</f>
         <v>0</v>
@@ -1858,7 +1839,7 @@
         <f>G57+G110</f>
         <v>0</v>
       </c>
-      <c r="H1" s="125" t="s">
+      <c r="H1" s="151" t="s">
         <v>11</v>
       </c>
       <c r="I1" s="20">
@@ -1873,16 +1854,16 @@
         <f>K57+K110</f>
         <v>0</v>
       </c>
-      <c r="L1" s="142"/>
-      <c r="M1" s="125" t="s">
+      <c r="L1" s="128"/>
+      <c r="M1" s="151" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="142"/>
+      <c r="N1" s="128"/>
       <c r="O1" s="20">
         <f>O57+O110</f>
         <v>0</v>
       </c>
-      <c r="P1" s="138" t="s">
+      <c r="P1" s="147" t="s">
         <v>72</v>
       </c>
       <c r="Q1" s="20">
@@ -1897,8 +1878,8 @@
         <f>S57+S110</f>
         <v>0</v>
       </c>
-      <c r="T1" s="142"/>
-      <c r="U1" s="133" t="s">
+      <c r="T1" s="128"/>
+      <c r="U1" s="143" t="s">
         <v>31</v>
       </c>
       <c r="V1" s="20">
@@ -1923,152 +1904,152 @@
       </c>
       <c r="AA1" s="21"/>
     </row>
-    <row r="2" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="124"/>
-      <c r="B2" s="134"/>
-      <c r="C2" s="135" t="s">
+    <row r="2" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="150"/>
+      <c r="B2" s="127"/>
+      <c r="C2" s="144" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="137" t="s">
+      <c r="D2" s="146" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="132" t="s">
+      <c r="E2" s="135" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="128" t="s">
+      <c r="F2" s="131" t="s">
         <v>56</v>
       </c>
-      <c r="G2" s="130" t="s">
+      <c r="G2" s="119" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="127"/>
-      <c r="I2" s="147" t="s">
+      <c r="H2" s="153"/>
+      <c r="I2" s="140" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="128" t="s">
+      <c r="J2" s="131" t="s">
         <v>56</v>
       </c>
-      <c r="K2" s="130" t="s">
+      <c r="K2" s="119" t="s">
         <v>58</v>
       </c>
-      <c r="L2" s="148"/>
-      <c r="M2" s="126"/>
-      <c r="N2" s="148"/>
-      <c r="O2" s="130" t="s">
+      <c r="L2" s="129"/>
+      <c r="M2" s="152"/>
+      <c r="N2" s="129"/>
+      <c r="O2" s="119" t="s">
         <v>59</v>
       </c>
-      <c r="P2" s="139"/>
-      <c r="Q2" s="130" t="s">
+      <c r="P2" s="148"/>
+      <c r="Q2" s="119" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="132" t="s">
+      <c r="R2" s="135" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="130" t="s">
+      <c r="S2" s="119" t="s">
         <v>60</v>
       </c>
-      <c r="T2" s="143"/>
-      <c r="U2" s="134"/>
-      <c r="V2" s="144" t="s">
+      <c r="T2" s="136"/>
+      <c r="U2" s="127"/>
+      <c r="V2" s="137" t="s">
         <v>29</v>
       </c>
-      <c r="W2" s="144" t="s">
+      <c r="W2" s="137" t="s">
         <v>30</v>
       </c>
-      <c r="X2" s="144" t="s">
+      <c r="X2" s="137" t="s">
         <v>32</v>
       </c>
-      <c r="Y2" s="132" t="s">
+      <c r="Y2" s="135" t="s">
         <v>50</v>
       </c>
-      <c r="Z2" s="132" t="s">
+      <c r="Z2" s="135" t="s">
         <v>51</v>
       </c>
       <c r="AA2" s="22"/>
     </row>
-    <row r="3" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="124"/>
-      <c r="B3" s="134"/>
-      <c r="C3" s="136"/>
-      <c r="D3" s="137"/>
-      <c r="E3" s="132"/>
-      <c r="F3" s="129"/>
-      <c r="G3" s="131"/>
-      <c r="H3" s="127"/>
-      <c r="I3" s="147"/>
-      <c r="J3" s="129"/>
-      <c r="K3" s="131"/>
-      <c r="L3" s="148"/>
-      <c r="M3" s="126"/>
-      <c r="N3" s="148"/>
-      <c r="O3" s="131"/>
-      <c r="P3" s="139"/>
-      <c r="Q3" s="150"/>
-      <c r="R3" s="132"/>
-      <c r="S3" s="131"/>
-      <c r="T3" s="143"/>
-      <c r="U3" s="134"/>
-      <c r="V3" s="132"/>
-      <c r="W3" s="132"/>
-      <c r="X3" s="132"/>
-      <c r="Y3" s="132"/>
-      <c r="Z3" s="132"/>
+    <row r="3" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="150"/>
+      <c r="B3" s="127"/>
+      <c r="C3" s="145"/>
+      <c r="D3" s="146"/>
+      <c r="E3" s="135"/>
+      <c r="F3" s="132"/>
+      <c r="G3" s="120"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="140"/>
+      <c r="J3" s="132"/>
+      <c r="K3" s="120"/>
+      <c r="L3" s="129"/>
+      <c r="M3" s="152"/>
+      <c r="N3" s="129"/>
+      <c r="O3" s="120"/>
+      <c r="P3" s="148"/>
+      <c r="Q3" s="141"/>
+      <c r="R3" s="135"/>
+      <c r="S3" s="120"/>
+      <c r="T3" s="136"/>
+      <c r="U3" s="127"/>
+      <c r="V3" s="135"/>
+      <c r="W3" s="135"/>
+      <c r="X3" s="135"/>
+      <c r="Y3" s="135"/>
+      <c r="Z3" s="135"/>
       <c r="AA3" s="22"/>
     </row>
-    <row r="4" spans="1:27" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="124"/>
-      <c r="B4" s="134"/>
-      <c r="C4" s="136"/>
-      <c r="D4" s="137"/>
-      <c r="E4" s="132"/>
+    <row r="4" spans="1:27" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="150"/>
+      <c r="B4" s="127"/>
+      <c r="C4" s="145"/>
+      <c r="D4" s="146"/>
+      <c r="E4" s="135"/>
       <c r="F4" s="112">
         <f>[1]Admin!$B$4</f>
-        <v>44292</v>
+        <v>44657</v>
       </c>
       <c r="G4" s="112">
         <f>[1]Admin!$B$4</f>
-        <v>44292</v>
-      </c>
-      <c r="H4" s="127"/>
-      <c r="I4" s="147"/>
+        <v>44657</v>
+      </c>
+      <c r="H4" s="153"/>
+      <c r="I4" s="140"/>
       <c r="J4" s="112">
         <f>[1]Admin!$B$17</f>
-        <v>44656</v>
+        <v>45021</v>
       </c>
       <c r="K4" s="112">
         <f>[1]Admin!$B$17</f>
-        <v>44656</v>
-      </c>
-      <c r="L4" s="149"/>
-      <c r="M4" s="126"/>
-      <c r="N4" s="149"/>
+        <v>45021</v>
+      </c>
+      <c r="L4" s="130"/>
+      <c r="M4" s="152"/>
+      <c r="N4" s="130"/>
       <c r="O4" s="112">
         <f>[1]Admin!$B$4</f>
-        <v>44292</v>
+        <v>44657</v>
       </c>
       <c r="P4" s="116">
         <f>[1]Admin!$G$4</f>
         <v>1</v>
       </c>
-      <c r="Q4" s="151"/>
+      <c r="Q4" s="142"/>
       <c r="R4" s="15">
         <f>[1]Admin!$G$5</f>
         <v>0.18</v>
       </c>
       <c r="S4" s="112">
         <f>[1]Admin!$B$17</f>
-        <v>44656</v>
-      </c>
-      <c r="T4" s="143"/>
-      <c r="U4" s="134"/>
-      <c r="V4" s="132"/>
-      <c r="W4" s="132"/>
-      <c r="X4" s="132"/>
-      <c r="Y4" s="132"/>
-      <c r="Z4" s="132"/>
+        <v>45021</v>
+      </c>
+      <c r="T4" s="136"/>
+      <c r="U4" s="127"/>
+      <c r="V4" s="135"/>
+      <c r="W4" s="135"/>
+      <c r="X4" s="135"/>
+      <c r="Y4" s="135"/>
+      <c r="Z4" s="135"/>
       <c r="AA4" s="23"/>
     </row>
-    <row r="5" spans="1:27" s="16" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" s="16" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A5" s="100"/>
       <c r="B5" s="55"/>
       <c r="C5" s="74"/>
@@ -2097,15 +2078,15 @@
       <c r="Z5" s="57"/>
       <c r="AA5" s="23"/>
     </row>
-    <row r="6" spans="1:27" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="101"/>
-      <c r="B6" s="152" t="s">
+      <c r="B6" s="117" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="154"/>
+      <c r="C6" s="121"/>
       <c r="D6" s="113">
         <f>[1]Admin!$B$4</f>
-        <v>44292</v>
+        <v>44657</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
@@ -2131,12 +2112,12 @@
       <c r="Z6" s="11"/>
       <c r="AA6" s="22"/>
     </row>
-    <row r="7" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="101"/>
-      <c r="B7" s="122" t="s">
+      <c r="B7" s="123" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="122"/>
+      <c r="C7" s="123"/>
       <c r="D7" s="30"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
@@ -2165,7 +2146,7 @@
       <c r="Z7" s="11"/>
       <c r="AA7" s="22"/>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A8" s="101"/>
       <c r="B8" s="42"/>
       <c r="C8" s="75"/>
@@ -2215,7 +2196,7 @@
       <c r="Z8" s="11"/>
       <c r="AA8" s="22"/>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A9" s="101"/>
       <c r="B9" s="42"/>
       <c r="C9" s="75"/>
@@ -2265,7 +2246,7 @@
       <c r="Z9" s="11"/>
       <c r="AA9" s="22"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A10" s="101"/>
       <c r="B10" s="42"/>
       <c r="C10" s="75"/>
@@ -2315,13 +2296,13 @@
       <c r="Z10" s="11"/>
       <c r="AA10" s="22"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A11" s="101"/>
-      <c r="B11" s="117" t="s">
+      <c r="B11" s="124" t="s">
         <v>67</v>
       </c>
-      <c r="C11" s="118"/>
-      <c r="D11" s="119"/>
+      <c r="C11" s="125"/>
+      <c r="D11" s="126"/>
       <c r="E11" s="41">
         <f>SUM(E8:E10)</f>
         <v>0</v>
@@ -2391,7 +2372,7 @@
       </c>
       <c r="AA11" s="22"/>
     </row>
-    <row r="12" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="101"/>
       <c r="B12" s="37"/>
       <c r="C12" s="76"/>
@@ -2420,12 +2401,12 @@
       <c r="Z12" s="7"/>
       <c r="AA12" s="22"/>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A13" s="101"/>
-      <c r="B13" s="122" t="s">
+      <c r="B13" s="123" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="122"/>
+      <c r="C13" s="123"/>
       <c r="D13" s="32"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
@@ -2454,7 +2435,7 @@
       <c r="Z13" s="11"/>
       <c r="AA13" s="22"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A14" s="101"/>
       <c r="B14" s="42"/>
       <c r="C14" s="75"/>
@@ -2516,7 +2497,7 @@
       </c>
       <c r="AA14" s="22"/>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A15" s="101"/>
       <c r="B15" s="42"/>
       <c r="C15" s="75"/>
@@ -2578,7 +2559,7 @@
       </c>
       <c r="AA15" s="22"/>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A16" s="101"/>
       <c r="B16" s="42"/>
       <c r="C16" s="75"/>
@@ -2640,7 +2621,7 @@
       </c>
       <c r="AA16" s="22"/>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A17" s="101"/>
       <c r="B17" s="42"/>
       <c r="C17" s="75"/>
@@ -2702,7 +2683,7 @@
       </c>
       <c r="AA17" s="22"/>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A18" s="101"/>
       <c r="B18" s="42"/>
       <c r="C18" s="75"/>
@@ -2764,13 +2745,13 @@
       </c>
       <c r="AA18" s="22"/>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A19" s="101"/>
-      <c r="B19" s="117" t="s">
+      <c r="B19" s="124" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="118"/>
-      <c r="D19" s="119"/>
+      <c r="C19" s="125"/>
+      <c r="D19" s="126"/>
       <c r="E19" s="41">
         <f>SUM(E14:E18)</f>
         <v>0</v>
@@ -2840,7 +2821,7 @@
       </c>
       <c r="AA19" s="22"/>
     </row>
-    <row r="20" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="101"/>
       <c r="B20" s="37"/>
       <c r="C20" s="76"/>
@@ -2869,12 +2850,12 @@
       <c r="Z20" s="7"/>
       <c r="AA20" s="22"/>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A21" s="101"/>
-      <c r="B21" s="122" t="s">
+      <c r="B21" s="123" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="122"/>
+      <c r="C21" s="123"/>
       <c r="D21" s="32"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
@@ -2903,7 +2884,7 @@
       <c r="Z21" s="11"/>
       <c r="AA21" s="22"/>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A22" s="101"/>
       <c r="B22" s="42"/>
       <c r="C22" s="75"/>
@@ -2965,7 +2946,7 @@
       </c>
       <c r="AA22" s="22"/>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A23" s="101"/>
       <c r="B23" s="42"/>
       <c r="C23" s="75"/>
@@ -3027,7 +3008,7 @@
       </c>
       <c r="AA23" s="22"/>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A24" s="101"/>
       <c r="B24" s="42"/>
       <c r="C24" s="75"/>
@@ -3089,7 +3070,7 @@
       </c>
       <c r="AA24" s="22"/>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A25" s="101"/>
       <c r="B25" s="42"/>
       <c r="C25" s="75"/>
@@ -3151,7 +3132,7 @@
       </c>
       <c r="AA25" s="22"/>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A26" s="101"/>
       <c r="B26" s="42"/>
       <c r="C26" s="75"/>
@@ -3213,13 +3194,13 @@
       </c>
       <c r="AA26" s="22"/>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A27" s="101"/>
-      <c r="B27" s="117" t="s">
+      <c r="B27" s="124" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="118"/>
-      <c r="D27" s="119"/>
+      <c r="C27" s="125"/>
+      <c r="D27" s="126"/>
       <c r="E27" s="41">
         <f>SUM(E22:E26)</f>
         <v>0</v>
@@ -3289,7 +3270,7 @@
       </c>
       <c r="AA27" s="22"/>
     </row>
-    <row r="28" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="101"/>
       <c r="B28" s="37"/>
       <c r="C28" s="76"/>
@@ -3318,12 +3299,12 @@
       <c r="Z28" s="7"/>
       <c r="AA28" s="22"/>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A29" s="101"/>
-      <c r="B29" s="122" t="s">
+      <c r="B29" s="123" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="122"/>
+      <c r="C29" s="123"/>
       <c r="D29" s="33"/>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
@@ -3352,7 +3333,7 @@
       <c r="Z29" s="11"/>
       <c r="AA29" s="22"/>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A30" s="101"/>
       <c r="B30" s="42"/>
       <c r="C30" s="75"/>
@@ -3414,7 +3395,7 @@
       </c>
       <c r="AA30" s="22"/>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A31" s="101"/>
       <c r="B31" s="42"/>
       <c r="C31" s="75"/>
@@ -3476,7 +3457,7 @@
       </c>
       <c r="AA31" s="22"/>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A32" s="101"/>
       <c r="B32" s="42"/>
       <c r="C32" s="75"/>
@@ -3538,7 +3519,7 @@
       </c>
       <c r="AA32" s="22"/>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A33" s="101"/>
       <c r="B33" s="42"/>
       <c r="C33" s="75"/>
@@ -3600,7 +3581,7 @@
       </c>
       <c r="AA33" s="22"/>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A34" s="101"/>
       <c r="B34" s="42"/>
       <c r="C34" s="75"/>
@@ -3662,13 +3643,13 @@
       </c>
       <c r="AA34" s="22"/>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A35" s="101"/>
-      <c r="B35" s="117" t="s">
+      <c r="B35" s="124" t="s">
         <v>70</v>
       </c>
-      <c r="C35" s="118"/>
-      <c r="D35" s="119"/>
+      <c r="C35" s="125"/>
+      <c r="D35" s="126"/>
       <c r="E35" s="41">
         <f>SUM(E30:E34)</f>
         <v>0</v>
@@ -3738,7 +3719,7 @@
       </c>
       <c r="AA35" s="22"/>
     </row>
-    <row r="36" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="101"/>
       <c r="B36" s="37"/>
       <c r="C36" s="76"/>
@@ -3767,12 +3748,12 @@
       <c r="Z36" s="7"/>
       <c r="AA36" s="22"/>
     </row>
-    <row r="37" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:27" ht="13" x14ac:dyDescent="0.15">
       <c r="A37" s="101"/>
-      <c r="B37" s="120" t="s">
+      <c r="B37" s="154" t="s">
         <v>63</v>
       </c>
-      <c r="C37" s="121"/>
+      <c r="C37" s="155"/>
       <c r="D37" s="114">
         <f>[1]Admin!$E$8</f>
         <v>12000</v>
@@ -3804,7 +3785,7 @@
       <c r="Z37" s="7"/>
       <c r="AA37" s="22"/>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A38" s="101"/>
       <c r="B38" s="42"/>
       <c r="C38" s="75"/>
@@ -3868,7 +3849,7 @@
       </c>
       <c r="AA38" s="22"/>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A39" s="101"/>
       <c r="B39" s="42"/>
       <c r="C39" s="75"/>
@@ -3932,7 +3913,7 @@
       </c>
       <c r="AA39" s="22"/>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A40" s="101"/>
       <c r="B40" s="42"/>
       <c r="C40" s="75"/>
@@ -3996,7 +3977,7 @@
       </c>
       <c r="AA40" s="22"/>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A41" s="101"/>
       <c r="B41" s="42"/>
       <c r="C41" s="75"/>
@@ -4060,7 +4041,7 @@
       </c>
       <c r="AA41" s="22"/>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A42" s="101"/>
       <c r="B42" s="42"/>
       <c r="C42" s="75"/>
@@ -4124,12 +4105,12 @@
       </c>
       <c r="AA42" s="22"/>
     </row>
-    <row r="43" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="101"/>
-      <c r="B43" s="120" t="s">
+      <c r="B43" s="154" t="s">
         <v>64</v>
       </c>
-      <c r="C43" s="121"/>
+      <c r="C43" s="155"/>
       <c r="D43" s="114">
         <f>[1]Admin!$E$8</f>
         <v>12000</v>
@@ -4158,7 +4139,7 @@
       <c r="Z43" s="11"/>
       <c r="AA43" s="22"/>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A44" s="101"/>
       <c r="B44" s="42"/>
       <c r="C44" s="75"/>
@@ -4222,7 +4203,7 @@
       </c>
       <c r="AA44" s="22"/>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A45" s="101"/>
       <c r="B45" s="42"/>
       <c r="C45" s="75"/>
@@ -4286,7 +4267,7 @@
       </c>
       <c r="AA45" s="22"/>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A46" s="101"/>
       <c r="B46" s="42"/>
       <c r="C46" s="75"/>
@@ -4350,7 +4331,7 @@
       </c>
       <c r="AA46" s="22"/>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A47" s="101"/>
       <c r="B47" s="42"/>
       <c r="C47" s="75"/>
@@ -4414,7 +4395,7 @@
       </c>
       <c r="AA47" s="22"/>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A48" s="101"/>
       <c r="B48" s="42"/>
       <c r="C48" s="75"/>
@@ -4478,12 +4459,12 @@
       </c>
       <c r="AA48" s="22"/>
     </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A49" s="101"/>
-      <c r="B49" s="122" t="s">
+      <c r="B49" s="123" t="s">
         <v>54</v>
       </c>
-      <c r="C49" s="122"/>
+      <c r="C49" s="123"/>
       <c r="D49" s="32"/>
       <c r="E49" s="7"/>
       <c r="F49" s="7"/>
@@ -4509,7 +4490,7 @@
       <c r="Z49" s="11"/>
       <c r="AA49" s="22"/>
     </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A50" s="101"/>
       <c r="B50" s="42"/>
       <c r="C50" s="75"/>
@@ -4573,7 +4554,7 @@
       </c>
       <c r="AA50" s="22"/>
     </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A51" s="101"/>
       <c r="B51" s="42"/>
       <c r="C51" s="75"/>
@@ -4637,7 +4618,7 @@
       </c>
       <c r="AA51" s="22"/>
     </row>
-    <row r="52" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A52" s="101"/>
       <c r="B52" s="42"/>
       <c r="C52" s="75"/>
@@ -4701,7 +4682,7 @@
       </c>
       <c r="AA52" s="22"/>
     </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A53" s="101"/>
       <c r="B53" s="42"/>
       <c r="C53" s="75"/>
@@ -4765,7 +4746,7 @@
       </c>
       <c r="AA53" s="22"/>
     </row>
-    <row r="54" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A54" s="101"/>
       <c r="B54" s="42"/>
       <c r="C54" s="75"/>
@@ -4829,13 +4810,13 @@
       </c>
       <c r="AA54" s="22"/>
     </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A55" s="101"/>
-      <c r="B55" s="117" t="s">
+      <c r="B55" s="124" t="s">
         <v>71</v>
       </c>
-      <c r="C55" s="118"/>
-      <c r="D55" s="119"/>
+      <c r="C55" s="125"/>
+      <c r="D55" s="126"/>
       <c r="E55" s="17">
         <f>SUM(E38:E54)</f>
         <v>0</v>
@@ -4905,7 +4886,7 @@
       </c>
       <c r="AA55" s="22"/>
     </row>
-    <row r="56" spans="1:27" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:27" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A56" s="101"/>
       <c r="B56" s="12"/>
       <c r="C56" s="77"/>
@@ -4934,16 +4915,16 @@
       <c r="Z56" s="11"/>
       <c r="AA56" s="22"/>
     </row>
-    <row r="57" spans="1:27" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:27" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A57" s="101"/>
-      <c r="B57" s="152" t="str">
+      <c r="B57" s="117" t="str">
         <f>B6</f>
         <v xml:space="preserve">EXISTING FIXED ASSETS at </v>
       </c>
-      <c r="C57" s="154"/>
+      <c r="C57" s="121"/>
       <c r="D57" s="113">
         <f>D6</f>
-        <v>44292</v>
+        <v>44657</v>
       </c>
       <c r="E57" s="19">
         <f>E11+E19+E27+E35+E55</f>
@@ -5014,7 +4995,7 @@
       </c>
       <c r="AA57" s="22"/>
     </row>
-    <row r="58" spans="1:27" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:27" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A58" s="101"/>
       <c r="B58" s="14"/>
       <c r="C58" s="78"/>
@@ -5043,19 +5024,19 @@
       <c r="Z58" s="11"/>
       <c r="AA58" s="22"/>
     </row>
-    <row r="59" spans="1:27" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:27" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A59" s="101"/>
-      <c r="B59" s="152" t="s">
+      <c r="B59" s="117" t="s">
         <v>62</v>
       </c>
-      <c r="C59" s="153"/>
+      <c r="C59" s="118"/>
       <c r="D59" s="113">
         <f>[1]Admin!$B$4</f>
-        <v>44292</v>
+        <v>44657</v>
       </c>
       <c r="E59" s="11"/>
-      <c r="F59" s="140"/>
-      <c r="G59" s="141"/>
+      <c r="F59" s="133"/>
+      <c r="G59" s="134"/>
       <c r="H59" s="13"/>
       <c r="I59" s="11"/>
       <c r="J59" s="11"/>
@@ -5077,16 +5058,16 @@
       <c r="Z59" s="11"/>
       <c r="AA59" s="22"/>
     </row>
-    <row r="60" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="101"/>
-      <c r="B60" s="122" t="s">
+      <c r="B60" s="123" t="s">
         <v>10</v>
       </c>
-      <c r="C60" s="122"/>
+      <c r="C60" s="123"/>
       <c r="D60" s="30"/>
       <c r="E60" s="8"/>
-      <c r="F60" s="141"/>
-      <c r="G60" s="141"/>
+      <c r="F60" s="134"/>
+      <c r="G60" s="134"/>
       <c r="H60" s="39">
         <f>H$7</f>
         <v>0</v>
@@ -5111,7 +5092,7 @@
       <c r="Z60" s="11"/>
       <c r="AA60" s="22"/>
     </row>
-    <row r="61" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A61" s="101"/>
       <c r="B61" s="42"/>
       <c r="C61" s="75"/>
@@ -5158,7 +5139,7 @@
       <c r="Z61" s="11"/>
       <c r="AA61" s="22"/>
     </row>
-    <row r="62" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A62" s="101"/>
       <c r="B62" s="42"/>
       <c r="C62" s="75"/>
@@ -5205,7 +5186,7 @@
       <c r="Z62" s="11"/>
       <c r="AA62" s="22"/>
     </row>
-    <row r="63" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A63" s="101"/>
       <c r="B63" s="42"/>
       <c r="C63" s="75"/>
@@ -5252,13 +5233,13 @@
       <c r="Z63" s="11"/>
       <c r="AA63" s="22"/>
     </row>
-    <row r="64" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A64" s="101"/>
-      <c r="B64" s="117" t="s">
+      <c r="B64" s="124" t="s">
         <v>12</v>
       </c>
-      <c r="C64" s="118"/>
-      <c r="D64" s="119"/>
+      <c r="C64" s="125"/>
+      <c r="D64" s="126"/>
       <c r="E64" s="41">
         <f>SUM(E61:E63)</f>
         <v>0</v>
@@ -5328,7 +5309,7 @@
       </c>
       <c r="AA64" s="22"/>
     </row>
-    <row r="65" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="101"/>
       <c r="B65" s="37"/>
       <c r="C65" s="76"/>
@@ -5357,12 +5338,12 @@
       <c r="Z65" s="7"/>
       <c r="AA65" s="22"/>
     </row>
-    <row r="66" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="101"/>
-      <c r="B66" s="122" t="s">
+      <c r="B66" s="123" t="s">
         <v>9</v>
       </c>
-      <c r="C66" s="122"/>
+      <c r="C66" s="123"/>
       <c r="D66" s="32"/>
       <c r="E66" s="7"/>
       <c r="F66" s="7"/>
@@ -5391,7 +5372,7 @@
       <c r="Z66" s="11"/>
       <c r="AA66" s="22"/>
     </row>
-    <row r="67" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A67" s="101"/>
       <c r="B67" s="42"/>
       <c r="C67" s="75"/>
@@ -5453,7 +5434,7 @@
       </c>
       <c r="AA67" s="22"/>
     </row>
-    <row r="68" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A68" s="101"/>
       <c r="B68" s="42"/>
       <c r="C68" s="75"/>
@@ -5515,7 +5496,7 @@
       </c>
       <c r="AA68" s="22"/>
     </row>
-    <row r="69" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A69" s="101"/>
       <c r="B69" s="42"/>
       <c r="C69" s="75"/>
@@ -5577,7 +5558,7 @@
       </c>
       <c r="AA69" s="22"/>
     </row>
-    <row r="70" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A70" s="101"/>
       <c r="B70" s="42"/>
       <c r="C70" s="75"/>
@@ -5639,7 +5620,7 @@
       </c>
       <c r="AA70" s="22"/>
     </row>
-    <row r="71" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A71" s="101"/>
       <c r="B71" s="42"/>
       <c r="C71" s="75"/>
@@ -5701,13 +5682,13 @@
       </c>
       <c r="AA71" s="22"/>
     </row>
-    <row r="72" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A72" s="101"/>
-      <c r="B72" s="117" t="s">
+      <c r="B72" s="124" t="s">
         <v>13</v>
       </c>
-      <c r="C72" s="118"/>
-      <c r="D72" s="119"/>
+      <c r="C72" s="125"/>
+      <c r="D72" s="126"/>
       <c r="E72" s="41">
         <f>SUM(E67:E71)</f>
         <v>0</v>
@@ -5777,7 +5758,7 @@
       </c>
       <c r="AA72" s="22"/>
     </row>
-    <row r="73" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="101"/>
       <c r="B73" s="37"/>
       <c r="C73" s="76"/>
@@ -5806,12 +5787,12 @@
       <c r="Z73" s="7"/>
       <c r="AA73" s="22"/>
     </row>
-    <row r="74" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A74" s="101"/>
-      <c r="B74" s="122" t="s">
+      <c r="B74" s="123" t="s">
         <v>55</v>
       </c>
-      <c r="C74" s="122"/>
+      <c r="C74" s="123"/>
       <c r="D74" s="32"/>
       <c r="E74" s="7"/>
       <c r="F74" s="7"/>
@@ -5840,7 +5821,7 @@
       <c r="Z74" s="11"/>
       <c r="AA74" s="22"/>
     </row>
-    <row r="75" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="101"/>
       <c r="B75" s="42"/>
       <c r="C75" s="75"/>
@@ -5902,7 +5883,7 @@
       </c>
       <c r="AA75" s="22"/>
     </row>
-    <row r="76" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A76" s="101"/>
       <c r="B76" s="42"/>
       <c r="C76" s="75"/>
@@ -5964,7 +5945,7 @@
       </c>
       <c r="AA76" s="22"/>
     </row>
-    <row r="77" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A77" s="101"/>
       <c r="B77" s="42"/>
       <c r="C77" s="75"/>
@@ -6026,7 +6007,7 @@
       </c>
       <c r="AA77" s="22"/>
     </row>
-    <row r="78" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A78" s="101"/>
       <c r="B78" s="42"/>
       <c r="C78" s="75"/>
@@ -6088,7 +6069,7 @@
       </c>
       <c r="AA78" s="22"/>
     </row>
-    <row r="79" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A79" s="101"/>
       <c r="B79" s="42"/>
       <c r="C79" s="75"/>
@@ -6150,13 +6131,13 @@
       </c>
       <c r="AA79" s="22"/>
     </row>
-    <row r="80" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A80" s="101"/>
-      <c r="B80" s="117" t="s">
+      <c r="B80" s="124" t="s">
         <v>14</v>
       </c>
-      <c r="C80" s="118"/>
-      <c r="D80" s="119"/>
+      <c r="C80" s="125"/>
+      <c r="D80" s="126"/>
       <c r="E80" s="41">
         <f>SUM(E75:E79)</f>
         <v>0</v>
@@ -6226,7 +6207,7 @@
       </c>
       <c r="AA80" s="22"/>
     </row>
-    <row r="81" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="101"/>
       <c r="B81" s="37"/>
       <c r="C81" s="76"/>
@@ -6255,12 +6236,12 @@
       <c r="Z81" s="7"/>
       <c r="AA81" s="22"/>
     </row>
-    <row r="82" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A82" s="101"/>
-      <c r="B82" s="122" t="s">
+      <c r="B82" s="123" t="s">
         <v>7</v>
       </c>
-      <c r="C82" s="122"/>
+      <c r="C82" s="123"/>
       <c r="D82" s="33"/>
       <c r="E82" s="7"/>
       <c r="F82" s="7"/>
@@ -6289,7 +6270,7 @@
       <c r="Z82" s="11"/>
       <c r="AA82" s="22"/>
     </row>
-    <row r="83" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A83" s="101"/>
       <c r="B83" s="42"/>
       <c r="C83" s="75"/>
@@ -6351,7 +6332,7 @@
       </c>
       <c r="AA83" s="22"/>
     </row>
-    <row r="84" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A84" s="101"/>
       <c r="B84" s="42"/>
       <c r="C84" s="75"/>
@@ -6413,7 +6394,7 @@
       </c>
       <c r="AA84" s="22"/>
     </row>
-    <row r="85" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A85" s="101"/>
       <c r="B85" s="42"/>
       <c r="C85" s="75"/>
@@ -6475,7 +6456,7 @@
       </c>
       <c r="AA85" s="22"/>
     </row>
-    <row r="86" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A86" s="101"/>
       <c r="B86" s="42"/>
       <c r="C86" s="75"/>
@@ -6537,7 +6518,7 @@
       </c>
       <c r="AA86" s="22"/>
     </row>
-    <row r="87" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A87" s="101"/>
       <c r="B87" s="42"/>
       <c r="C87" s="75"/>
@@ -6599,13 +6580,13 @@
       </c>
       <c r="AA87" s="22"/>
     </row>
-    <row r="88" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A88" s="101"/>
-      <c r="B88" s="117" t="s">
+      <c r="B88" s="124" t="s">
         <v>15</v>
       </c>
-      <c r="C88" s="118"/>
-      <c r="D88" s="119"/>
+      <c r="C88" s="125"/>
+      <c r="D88" s="126"/>
       <c r="E88" s="41">
         <f>SUM(E83:E87)</f>
         <v>0</v>
@@ -6675,7 +6656,7 @@
       </c>
       <c r="AA88" s="22"/>
     </row>
-    <row r="89" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A89" s="101"/>
       <c r="B89" s="37"/>
       <c r="C89" s="76"/>
@@ -6704,13 +6685,13 @@
       <c r="Z89" s="7"/>
       <c r="AA89" s="22"/>
     </row>
-    <row r="90" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A90" s="101"/>
-      <c r="B90" s="120" t="str">
+      <c r="B90" s="154" t="str">
         <f>B37</f>
         <v>Motor Vehicles - costing over £</v>
       </c>
-      <c r="C90" s="120"/>
+      <c r="C90" s="154"/>
       <c r="D90" s="114">
         <f>D37</f>
         <v>12000</v>
@@ -6742,7 +6723,7 @@
       <c r="Z90" s="11"/>
       <c r="AA90" s="22"/>
     </row>
-    <row r="91" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A91" s="101"/>
       <c r="B91" s="42"/>
       <c r="C91" s="75"/>
@@ -6803,7 +6784,7 @@
       </c>
       <c r="AA91" s="22"/>
     </row>
-    <row r="92" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A92" s="101"/>
       <c r="B92" s="42"/>
       <c r="C92" s="75"/>
@@ -6864,7 +6845,7 @@
       </c>
       <c r="AA92" s="22"/>
     </row>
-    <row r="93" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A93" s="101"/>
       <c r="B93" s="42"/>
       <c r="C93" s="75"/>
@@ -6925,7 +6906,7 @@
       </c>
       <c r="AA93" s="22"/>
     </row>
-    <row r="94" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A94" s="101"/>
       <c r="B94" s="42"/>
       <c r="C94" s="75"/>
@@ -6986,7 +6967,7 @@
       </c>
       <c r="AA94" s="22"/>
     </row>
-    <row r="95" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A95" s="101"/>
       <c r="B95" s="42"/>
       <c r="C95" s="75"/>
@@ -7047,13 +7028,13 @@
       </c>
       <c r="AA95" s="22"/>
     </row>
-    <row r="96" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A96" s="101"/>
-      <c r="B96" s="155" t="str">
+      <c r="B96" s="122" t="str">
         <f>B43</f>
         <v>Motor Vehicles - costing under £</v>
       </c>
-      <c r="C96" s="155"/>
+      <c r="C96" s="122"/>
       <c r="D96" s="114">
         <f>D43</f>
         <v>12000</v>
@@ -7082,7 +7063,7 @@
       <c r="Z96" s="11"/>
       <c r="AA96" s="22"/>
     </row>
-    <row r="97" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A97" s="101"/>
       <c r="B97" s="42"/>
       <c r="C97" s="75"/>
@@ -7143,7 +7124,7 @@
       </c>
       <c r="AA97" s="22"/>
     </row>
-    <row r="98" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A98" s="101"/>
       <c r="B98" s="42"/>
       <c r="C98" s="75"/>
@@ -7204,7 +7185,7 @@
       </c>
       <c r="AA98" s="22"/>
     </row>
-    <row r="99" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A99" s="101"/>
       <c r="B99" s="42"/>
       <c r="C99" s="75"/>
@@ -7265,7 +7246,7 @@
       </c>
       <c r="AA99" s="22"/>
     </row>
-    <row r="100" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A100" s="101"/>
       <c r="B100" s="42"/>
       <c r="C100" s="75"/>
@@ -7326,7 +7307,7 @@
       </c>
       <c r="AA100" s="22"/>
     </row>
-    <row r="101" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A101" s="101"/>
       <c r="B101" s="42"/>
       <c r="C101" s="75"/>
@@ -7387,12 +7368,12 @@
       </c>
       <c r="AA101" s="22"/>
     </row>
-    <row r="102" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A102" s="101"/>
-      <c r="B102" s="122" t="s">
+      <c r="B102" s="123" t="s">
         <v>54</v>
       </c>
-      <c r="C102" s="122"/>
+      <c r="C102" s="123"/>
       <c r="D102" s="33"/>
       <c r="E102" s="7"/>
       <c r="F102" s="7"/>
@@ -7418,7 +7399,7 @@
       <c r="Z102" s="11"/>
       <c r="AA102" s="22"/>
     </row>
-    <row r="103" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A103" s="101"/>
       <c r="B103" s="42"/>
       <c r="C103" s="75"/>
@@ -7482,7 +7463,7 @@
       </c>
       <c r="AA103" s="22"/>
     </row>
-    <row r="104" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A104" s="101"/>
       <c r="B104" s="42"/>
       <c r="C104" s="75"/>
@@ -7546,7 +7527,7 @@
       </c>
       <c r="AA104" s="22"/>
     </row>
-    <row r="105" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A105" s="101"/>
       <c r="B105" s="42"/>
       <c r="C105" s="75"/>
@@ -7610,7 +7591,7 @@
       </c>
       <c r="AA105" s="22"/>
     </row>
-    <row r="106" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A106" s="101"/>
       <c r="B106" s="42"/>
       <c r="C106" s="75"/>
@@ -7674,7 +7655,7 @@
       </c>
       <c r="AA106" s="22"/>
     </row>
-    <row r="107" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A107" s="101"/>
       <c r="B107" s="42"/>
       <c r="C107" s="75"/>
@@ -7738,13 +7719,13 @@
       </c>
       <c r="AA107" s="22"/>
     </row>
-    <row r="108" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A108" s="101"/>
-      <c r="B108" s="117" t="s">
+      <c r="B108" s="124" t="s">
         <v>16</v>
       </c>
-      <c r="C108" s="118"/>
-      <c r="D108" s="119"/>
+      <c r="C108" s="125"/>
+      <c r="D108" s="126"/>
       <c r="E108" s="17">
         <f>SUM(E91:E107)</f>
         <v>0</v>
@@ -7814,7 +7795,7 @@
       </c>
       <c r="AA108" s="22"/>
     </row>
-    <row r="109" spans="1:27" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:27" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A109" s="101"/>
       <c r="B109" s="12"/>
       <c r="C109" s="77"/>
@@ -7843,16 +7824,16 @@
       <c r="Z109" s="11"/>
       <c r="AA109" s="22"/>
     </row>
-    <row r="110" spans="1:27" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:27" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A110" s="101"/>
-      <c r="B110" s="152" t="str">
+      <c r="B110" s="117" t="str">
         <f>B59</f>
         <v xml:space="preserve">NEW FIXED ASSETS Bought AFTER </v>
       </c>
-      <c r="C110" s="153"/>
+      <c r="C110" s="118"/>
       <c r="D110" s="113">
         <f>D59</f>
-        <v>44292</v>
+        <v>44657</v>
       </c>
       <c r="E110" s="19">
         <f>E64+E72+E80+E88+E108</f>
@@ -7923,7 +7904,7 @@
       </c>
       <c r="AA110" s="22"/>
     </row>
-    <row r="111" spans="1:27" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:27" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A111" s="102"/>
       <c r="B111" s="24"/>
       <c r="C111" s="79"/>
@@ -7954,6 +7935,46 @@
     </row>
   </sheetData>
   <mergeCells count="56">
+    <mergeCell ref="B108:D108"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B102:C102"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B88:D88"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="B72:D72"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="M1:M4"/>
+    <mergeCell ref="H1:H4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="U1:U4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="P1:P3"/>
+    <mergeCell ref="F59:G60"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="T1:T4"/>
+    <mergeCell ref="X2:X4"/>
+    <mergeCell ref="V2:V4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="L1:L4"/>
+    <mergeCell ref="Q2:Q4"/>
+    <mergeCell ref="O2:O3"/>
     <mergeCell ref="B110:C110"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="B6:C6"/>
@@ -7970,46 +7991,6 @@
     <mergeCell ref="N1:N4"/>
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="K2:K3"/>
-    <mergeCell ref="F59:G60"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="T1:T4"/>
-    <mergeCell ref="X2:X4"/>
-    <mergeCell ref="V2:V4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="I2:I4"/>
-    <mergeCell ref="L1:L4"/>
-    <mergeCell ref="Q2:Q4"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="U1:U4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="P1:P3"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="M1:M4"/>
-    <mergeCell ref="H1:H4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="B108:D108"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B102:C102"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B88:D88"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="B72:D72"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="B66:C66"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -8039,38 +8020,39 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="1.7109375" style="104" customWidth="1"/>
-    <col min="2" max="2" width="27.140625" style="104" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="104"/>
-    <col min="4" max="4" width="3.7109375" style="104" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="104" customWidth="1"/>
-    <col min="6" max="6" width="5.42578125" style="104" customWidth="1"/>
-    <col min="7" max="9" width="9.140625" style="104"/>
-    <col min="10" max="10" width="6.5703125" style="104" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" style="104" customWidth="1"/>
-    <col min="12" max="12" width="2.7109375" style="104" customWidth="1"/>
-    <col min="13" max="14" width="9.7109375" style="104" customWidth="1"/>
-    <col min="15" max="15" width="1.5703125" style="104" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="104"/>
+    <col min="1" max="1" width="1.6640625" style="104" customWidth="1"/>
+    <col min="2" max="2" width="27.1640625" style="104" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" style="104"/>
+    <col min="4" max="4" width="3.6640625" style="104" customWidth="1"/>
+    <col min="5" max="5" width="11.5" style="104" customWidth="1"/>
+    <col min="6" max="6" width="5.5" style="104" customWidth="1"/>
+    <col min="7" max="9" width="9.1640625" style="104"/>
+    <col min="10" max="10" width="6.5" style="104" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" style="104" customWidth="1"/>
+    <col min="12" max="12" width="2.6640625" style="104" customWidth="1"/>
+    <col min="13" max="13" width="9.6640625" style="104" customWidth="1"/>
+    <col min="14" max="14" width="10.33203125" style="104" customWidth="1"/>
+    <col min="15" max="15" width="1.5" style="104" customWidth="1"/>
+    <col min="16" max="16384" width="9.1640625" style="104"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="5" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="165"/>
-      <c r="B1" s="166"/>
-      <c r="C1" s="166"/>
-      <c r="D1" s="166"/>
-      <c r="E1" s="166"/>
-      <c r="F1" s="166"/>
-      <c r="G1" s="166"/>
-      <c r="H1" s="166"/>
-      <c r="I1" s="166"/>
-      <c r="J1" s="166"/>
-      <c r="K1" s="166"/>
-      <c r="L1" s="166"/>
-      <c r="M1" s="166"/>
-      <c r="N1" s="166"/>
+    <row r="1" spans="1:24" s="5" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="156"/>
+      <c r="B1" s="157"/>
+      <c r="C1" s="157"/>
+      <c r="D1" s="157"/>
+      <c r="E1" s="157"/>
+      <c r="F1" s="157"/>
+      <c r="G1" s="157"/>
+      <c r="H1" s="157"/>
+      <c r="I1" s="157"/>
+      <c r="J1" s="157"/>
+      <c r="K1" s="157"/>
+      <c r="L1" s="157"/>
+      <c r="M1" s="157"/>
+      <c r="N1" s="157"/>
       <c r="O1" s="71"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
@@ -8082,17 +8064,17 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="64"/>
       <c r="B2" s="47"/>
       <c r="C2" s="48"/>
       <c r="D2" s="49"/>
-      <c r="E2" s="173" t="s">
+      <c r="E2" s="166" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="174"/>
-      <c r="G2" s="175"/>
-      <c r="H2" s="176"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="168"/>
+      <c r="H2" s="169"/>
       <c r="I2" s="50"/>
       <c r="J2" s="50"/>
       <c r="K2" s="50"/>
@@ -8110,7 +8092,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="64"/>
       <c r="B3" s="47"/>
       <c r="C3" s="48"/>
@@ -8136,7 +8118,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="64"/>
       <c r="B4" s="106" t="s">
         <v>65</v>
@@ -8147,20 +8129,20 @@
         <v>3</v>
       </c>
       <c r="F4" s="50"/>
-      <c r="G4" s="162" t="s">
+      <c r="G4" s="176" t="s">
         <v>52</v>
       </c>
-      <c r="H4" s="163"/>
-      <c r="I4" s="164"/>
+      <c r="H4" s="177"/>
+      <c r="I4" s="178"/>
       <c r="J4" s="50"/>
       <c r="K4" s="107" t="s">
         <v>27</v>
       </c>
       <c r="L4" s="50"/>
-      <c r="M4" s="159" t="s">
+      <c r="M4" s="173" t="s">
         <v>53</v>
       </c>
-      <c r="N4" s="160"/>
+      <c r="N4" s="174"/>
       <c r="O4" s="72"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
@@ -8172,7 +8154,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="64"/>
       <c r="B5" s="47" t="s">
         <v>19</v>
@@ -8189,8 +8171,8 @@
       <c r="J5" s="50"/>
       <c r="K5" s="50"/>
       <c r="L5" s="50"/>
-      <c r="M5" s="160"/>
-      <c r="N5" s="160"/>
+      <c r="M5" s="174"/>
+      <c r="N5" s="174"/>
       <c r="O5" s="72"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
@@ -8202,31 +8184,31 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="64"/>
-      <c r="B6" s="156" t="s">
+      <c r="B6" s="158" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="157"/>
-      <c r="D6" s="158"/>
+      <c r="C6" s="159"/>
+      <c r="D6" s="172"/>
       <c r="E6" s="53">
         <f>Schedule!E64</f>
         <v>0</v>
       </c>
       <c r="F6" s="50"/>
-      <c r="G6" s="156" t="s">
+      <c r="G6" s="158" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="157"/>
-      <c r="I6" s="157"/>
-      <c r="J6" s="167"/>
+      <c r="H6" s="159"/>
+      <c r="I6" s="159"/>
+      <c r="J6" s="160"/>
       <c r="K6" s="53">
         <f>Schedule!V11+Schedule!V64</f>
         <v>0</v>
       </c>
       <c r="L6" s="50"/>
-      <c r="M6" s="160"/>
-      <c r="N6" s="160"/>
+      <c r="M6" s="174"/>
+      <c r="N6" s="174"/>
       <c r="O6" s="72"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
@@ -8238,31 +8220,31 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="64"/>
-      <c r="B7" s="156" t="s">
+      <c r="B7" s="158" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="157"/>
-      <c r="D7" s="158"/>
+      <c r="C7" s="159"/>
+      <c r="D7" s="172"/>
       <c r="E7" s="53">
         <f>Schedule!E72</f>
         <v>0</v>
       </c>
       <c r="F7" s="50"/>
-      <c r="G7" s="156" t="s">
+      <c r="G7" s="158" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="157"/>
-      <c r="I7" s="157"/>
-      <c r="J7" s="167"/>
+      <c r="H7" s="159"/>
+      <c r="I7" s="159"/>
+      <c r="J7" s="160"/>
       <c r="K7" s="53">
         <f>Schedule!V19+Schedule!V72</f>
         <v>0</v>
       </c>
       <c r="L7" s="50"/>
-      <c r="M7" s="160"/>
-      <c r="N7" s="160"/>
+      <c r="M7" s="174"/>
+      <c r="N7" s="174"/>
       <c r="O7" s="72"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
@@ -8274,31 +8256,31 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="64"/>
-      <c r="B8" s="156" t="s">
+      <c r="B8" s="158" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="157"/>
-      <c r="D8" s="158"/>
+      <c r="C8" s="159"/>
+      <c r="D8" s="172"/>
       <c r="E8" s="53">
         <f>Schedule!E80</f>
         <v>0</v>
       </c>
       <c r="F8" s="50"/>
-      <c r="G8" s="156" t="s">
+      <c r="G8" s="158" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="157"/>
-      <c r="I8" s="157"/>
-      <c r="J8" s="167"/>
+      <c r="H8" s="159"/>
+      <c r="I8" s="159"/>
+      <c r="J8" s="160"/>
       <c r="K8" s="53">
         <f>Schedule!V27+Schedule!V80</f>
         <v>0</v>
       </c>
       <c r="L8" s="50"/>
-      <c r="M8" s="160"/>
-      <c r="N8" s="160"/>
+      <c r="M8" s="174"/>
+      <c r="N8" s="174"/>
       <c r="O8" s="72"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
@@ -8310,31 +8292,31 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" spans="1:24" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="64"/>
-      <c r="B9" s="156" t="s">
+      <c r="B9" s="158" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="157"/>
-      <c r="D9" s="158"/>
+      <c r="C9" s="159"/>
+      <c r="D9" s="172"/>
       <c r="E9" s="53">
         <f>Schedule!E88</f>
         <v>0</v>
       </c>
       <c r="F9" s="50"/>
-      <c r="G9" s="156" t="s">
+      <c r="G9" s="158" t="s">
         <v>25</v>
       </c>
-      <c r="H9" s="157"/>
-      <c r="I9" s="157"/>
-      <c r="J9" s="167"/>
+      <c r="H9" s="159"/>
+      <c r="I9" s="159"/>
+      <c r="J9" s="160"/>
       <c r="K9" s="53">
         <f>Schedule!V35+Schedule!V88</f>
         <v>0</v>
       </c>
       <c r="L9" s="50"/>
-      <c r="M9" s="160"/>
-      <c r="N9" s="160"/>
+      <c r="M9" s="174"/>
+      <c r="N9" s="174"/>
       <c r="O9" s="72"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
@@ -8346,31 +8328,31 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
     </row>
-    <row r="10" spans="1:24" s="5" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" s="5" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A10" s="64"/>
-      <c r="B10" s="156" t="s">
+      <c r="B10" s="158" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="157"/>
-      <c r="D10" s="158"/>
+      <c r="C10" s="159"/>
+      <c r="D10" s="172"/>
       <c r="E10" s="53">
         <f>Schedule!E108</f>
         <v>0</v>
       </c>
       <c r="F10" s="50"/>
-      <c r="G10" s="156" t="s">
+      <c r="G10" s="158" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="157"/>
-      <c r="I10" s="157"/>
-      <c r="J10" s="167"/>
+      <c r="H10" s="159"/>
+      <c r="I10" s="159"/>
+      <c r="J10" s="160"/>
       <c r="K10" s="53">
         <f>Schedule!V55+Schedule!V108</f>
         <v>0</v>
       </c>
       <c r="L10" s="50"/>
-      <c r="M10" s="160"/>
-      <c r="N10" s="160"/>
+      <c r="M10" s="174"/>
+      <c r="N10" s="174"/>
       <c r="O10" s="72"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
@@ -8382,31 +8364,31 @@
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
     </row>
-    <row r="11" spans="1:24" s="5" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" s="5" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="64"/>
-      <c r="B11" s="177" t="s">
+      <c r="B11" s="170" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="177"/>
-      <c r="D11" s="178"/>
+      <c r="C11" s="170"/>
+      <c r="D11" s="171"/>
       <c r="E11" s="54">
         <f>SUM(E6:E10)</f>
         <v>0</v>
       </c>
       <c r="F11" s="50"/>
-      <c r="G11" s="171" t="s">
+      <c r="G11" s="164" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="171"/>
-      <c r="I11" s="171"/>
-      <c r="J11" s="172"/>
+      <c r="H11" s="164"/>
+      <c r="I11" s="164"/>
+      <c r="J11" s="165"/>
       <c r="K11" s="54">
         <f>SUM(K6:K10)</f>
         <v>0</v>
       </c>
       <c r="L11" s="50"/>
-      <c r="M11" s="160"/>
-      <c r="N11" s="160"/>
+      <c r="M11" s="174"/>
+      <c r="N11" s="174"/>
       <c r="O11" s="72"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
@@ -8418,7 +8400,7 @@
       <c r="W11" s="2"/>
       <c r="X11" s="2"/>
     </row>
-    <row r="12" spans="1:24" s="5" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" s="5" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A12" s="64"/>
       <c r="B12" s="47"/>
       <c r="C12" s="48"/>
@@ -8431,8 +8413,8 @@
       <c r="J12" s="50"/>
       <c r="K12" s="50"/>
       <c r="L12" s="50"/>
-      <c r="M12" s="160"/>
-      <c r="N12" s="160"/>
+      <c r="M12" s="174"/>
+      <c r="N12" s="174"/>
       <c r="O12" s="72"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
@@ -8444,31 +8426,31 @@
       <c r="W12" s="2"/>
       <c r="X12" s="2"/>
     </row>
-    <row r="13" spans="1:24" s="5" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" s="5" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A13" s="64"/>
-      <c r="B13" s="177" t="s">
+      <c r="B13" s="170" t="s">
         <v>66</v>
       </c>
-      <c r="C13" s="177"/>
-      <c r="D13" s="178"/>
+      <c r="C13" s="170"/>
+      <c r="D13" s="171"/>
       <c r="E13" s="115">
-        <f>[2]Mar22!$AG$2</f>
+        <f>[2]Mar23!$AG$2</f>
         <v>0</v>
       </c>
       <c r="F13" s="50"/>
-      <c r="G13" s="171" t="s">
+      <c r="G13" s="164" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="171"/>
-      <c r="I13" s="171"/>
-      <c r="J13" s="172"/>
+      <c r="H13" s="164"/>
+      <c r="I13" s="164"/>
+      <c r="J13" s="165"/>
       <c r="K13" s="115">
-        <f>[3]Mar22!$AA$2</f>
+        <f>[3]Mar23!$AA$2</f>
         <v>0</v>
       </c>
       <c r="L13" s="50"/>
-      <c r="M13" s="161"/>
-      <c r="N13" s="161"/>
+      <c r="M13" s="175"/>
+      <c r="N13" s="175"/>
       <c r="O13" s="72"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
@@ -8480,7 +8462,7 @@
       <c r="W13" s="2"/>
       <c r="X13" s="2"/>
     </row>
-    <row r="14" spans="1:24" s="5" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" s="5" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A14" s="64"/>
       <c r="B14" s="47"/>
       <c r="C14" s="48"/>
@@ -8493,8 +8475,8 @@
       <c r="J14" s="50"/>
       <c r="K14" s="50"/>
       <c r="L14" s="50"/>
-      <c r="M14" s="161"/>
-      <c r="N14" s="161"/>
+      <c r="M14" s="175"/>
+      <c r="N14" s="175"/>
       <c r="O14" s="72"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
@@ -8506,33 +8488,33 @@
       <c r="W14" s="2"/>
       <c r="X14" s="2"/>
     </row>
-    <row r="15" spans="1:24" s="5" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" s="5" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A15" s="64"/>
-      <c r="B15" s="168" t="str">
+      <c r="B15" s="161" t="str">
         <f>IF(E15&gt;0,"Purchases exceed Assets listed on Schedule",IF(E15&lt;0,"Assets listed on Schedule exceed Purchase values","Purchases reconcile with Fixed asset Schedule"))</f>
         <v>Purchases reconcile with Fixed asset Schedule</v>
       </c>
-      <c r="C15" s="169"/>
-      <c r="D15" s="170"/>
+      <c r="C15" s="162"/>
+      <c r="D15" s="163"/>
       <c r="E15" s="105">
         <f>E13-E11</f>
         <v>0</v>
       </c>
       <c r="F15" s="50"/>
-      <c r="G15" s="168" t="str">
+      <c r="G15" s="161" t="str">
         <f>IF(K15&gt;0,"Sales exceed Assets listed on Schedule",IF(K15&lt;0,"Assets listed on Schedule exceed Sales values","Sales reconcile with Fixed asset Schedule"))</f>
         <v>Sales reconcile with Fixed asset Schedule</v>
       </c>
-      <c r="H15" s="169"/>
-      <c r="I15" s="169"/>
-      <c r="J15" s="170"/>
+      <c r="H15" s="162"/>
+      <c r="I15" s="162"/>
+      <c r="J15" s="163"/>
       <c r="K15" s="105">
         <f>K13-K11</f>
         <v>0</v>
       </c>
       <c r="L15" s="50"/>
-      <c r="M15" s="161"/>
-      <c r="N15" s="161"/>
+      <c r="M15" s="175"/>
+      <c r="N15" s="175"/>
       <c r="O15" s="72"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
@@ -8544,7 +8526,7 @@
       <c r="W15" s="2"/>
       <c r="X15" s="2"/>
     </row>
-    <row r="16" spans="1:24" s="5" customFormat="1" ht="9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" s="5" customFormat="1" ht="9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A16" s="65"/>
       <c r="B16" s="66"/>
       <c r="C16" s="67"/>
@@ -8572,6 +8554,10 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="M4:N15"/>
+    <mergeCell ref="G4:I4"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="G6:J6"/>
     <mergeCell ref="G15:J15"/>
@@ -8588,10 +8574,6 @@
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="M4:N15"/>
-    <mergeCell ref="G4:I4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -8614,21 +8596,21 @@
       <selection activeCell="C2" sqref="C2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="1.42578125" style="83" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="4" customWidth="1"/>
-    <col min="3" max="4" width="18.7109375" style="31" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="83" customWidth="1"/>
-    <col min="6" max="7" width="8.7109375" style="83" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" style="89" customWidth="1"/>
-    <col min="9" max="11" width="8.7109375" style="87" customWidth="1"/>
-    <col min="12" max="12" width="18.7109375" style="31" customWidth="1"/>
-    <col min="13" max="13" width="1.42578125" style="83" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="83"/>
+    <col min="1" max="1" width="1.5" style="83" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="4" customWidth="1"/>
+    <col min="3" max="4" width="18.6640625" style="31" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" style="83" customWidth="1"/>
+    <col min="6" max="7" width="8.6640625" style="83" customWidth="1"/>
+    <col min="8" max="8" width="6.6640625" style="89" customWidth="1"/>
+    <col min="9" max="11" width="8.6640625" style="87" customWidth="1"/>
+    <col min="12" max="12" width="18.6640625" style="31" customWidth="1"/>
+    <col min="13" max="13" width="1.5" style="83" customWidth="1"/>
+    <col min="14" max="16384" width="9.1640625" style="83"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="6" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="91"/>
       <c r="B1" s="47"/>
       <c r="C1" s="49"/>
@@ -8643,29 +8625,29 @@
       <c r="L1" s="49"/>
       <c r="M1" s="91"/>
     </row>
-    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="91"/>
       <c r="B2" s="81"/>
-      <c r="C2" s="183" t="s">
+      <c r="C2" s="184" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="184"/>
+      <c r="D2" s="185"/>
       <c r="E2" s="84">
         <f>SUM(E8:E14)</f>
         <v>0</v>
       </c>
       <c r="F2" s="82"/>
-      <c r="G2" s="179" t="s">
+      <c r="G2" s="182" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="180"/>
-      <c r="I2" s="180"/>
-      <c r="J2" s="180"/>
-      <c r="K2" s="180"/>
+      <c r="H2" s="183"/>
+      <c r="I2" s="183"/>
+      <c r="J2" s="183"/>
+      <c r="K2" s="183"/>
       <c r="L2" s="88"/>
       <c r="M2" s="91"/>
     </row>
-    <row r="3" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="91"/>
       <c r="B3" s="95" t="s">
         <v>40</v>
@@ -8674,15 +8656,15 @@
       <c r="D3" s="96"/>
       <c r="E3" s="82"/>
       <c r="F3" s="82"/>
-      <c r="G3" s="180"/>
-      <c r="H3" s="180"/>
-      <c r="I3" s="180"/>
-      <c r="J3" s="180"/>
-      <c r="K3" s="180"/>
+      <c r="G3" s="183"/>
+      <c r="H3" s="183"/>
+      <c r="I3" s="183"/>
+      <c r="J3" s="183"/>
+      <c r="K3" s="183"/>
       <c r="L3" s="88"/>
       <c r="M3" s="91"/>
     </row>
-    <row r="4" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="91"/>
       <c r="B4" s="12"/>
       <c r="C4" s="32"/>
@@ -8697,48 +8679,48 @@
       <c r="L4" s="97"/>
       <c r="M4" s="91"/>
     </row>
-    <row r="5" spans="1:13" s="86" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" s="86" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="94"/>
-      <c r="B5" s="134" t="s">
+      <c r="B5" s="127" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="137" t="s">
+      <c r="C5" s="146" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="137" t="s">
+      <c r="D5" s="146" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="181" t="s">
+      <c r="E5" s="180" t="s">
         <v>45</v>
       </c>
-      <c r="F5" s="181" t="s">
+      <c r="F5" s="180" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="181" t="s">
+      <c r="G5" s="180" t="s">
         <v>38</v>
       </c>
-      <c r="H5" s="137" t="s">
+      <c r="H5" s="146" t="s">
         <v>35</v>
       </c>
-      <c r="I5" s="181" t="s">
+      <c r="I5" s="180" t="s">
         <v>47</v>
       </c>
-      <c r="J5" s="182"/>
-      <c r="K5" s="182"/>
-      <c r="L5" s="137" t="s">
+      <c r="J5" s="181"/>
+      <c r="K5" s="181"/>
+      <c r="L5" s="146" t="s">
         <v>46</v>
       </c>
       <c r="M5" s="94"/>
     </row>
-    <row r="6" spans="1:13" s="86" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" s="86" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="94"/>
-      <c r="B6" s="185"/>
-      <c r="C6" s="185"/>
-      <c r="D6" s="185"/>
-      <c r="E6" s="185"/>
-      <c r="F6" s="185"/>
-      <c r="G6" s="185"/>
-      <c r="H6" s="185"/>
+      <c r="B6" s="179"/>
+      <c r="C6" s="179"/>
+      <c r="D6" s="179"/>
+      <c r="E6" s="179"/>
+      <c r="F6" s="179"/>
+      <c r="G6" s="179"/>
+      <c r="H6" s="179"/>
       <c r="I6" s="85" t="s">
         <v>34</v>
       </c>
@@ -8748,10 +8730,10 @@
       <c r="K6" s="85" t="s">
         <v>36</v>
       </c>
-      <c r="L6" s="185"/>
+      <c r="L6" s="179"/>
       <c r="M6" s="94"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A7" s="91"/>
       <c r="B7" s="12"/>
       <c r="C7" s="32"/>
@@ -8766,7 +8748,7 @@
       <c r="L7" s="32"/>
       <c r="M7" s="91"/>
     </row>
-    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="91"/>
       <c r="B8" s="42"/>
       <c r="C8" s="43"/>
@@ -8790,7 +8772,7 @@
       <c r="L8" s="43"/>
       <c r="M8" s="91"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A9" s="91"/>
       <c r="B9" s="12"/>
       <c r="C9" s="32"/>
@@ -8805,7 +8787,7 @@
       <c r="L9" s="32"/>
       <c r="M9" s="91"/>
     </row>
-    <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="91"/>
       <c r="B10" s="42"/>
       <c r="C10" s="43"/>
@@ -8829,7 +8811,7 @@
       <c r="L10" s="43"/>
       <c r="M10" s="91"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A11" s="91"/>
       <c r="B11" s="12"/>
       <c r="C11" s="32"/>
@@ -8844,7 +8826,7 @@
       <c r="L11" s="32"/>
       <c r="M11" s="91"/>
     </row>
-    <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="91"/>
       <c r="B12" s="42"/>
       <c r="C12" s="43"/>
@@ -8868,7 +8850,7 @@
       <c r="L12" s="43"/>
       <c r="M12" s="91"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A13" s="91"/>
       <c r="B13" s="12"/>
       <c r="C13" s="32"/>
@@ -8883,7 +8865,7 @@
       <c r="L13" s="32"/>
       <c r="M13" s="91"/>
     </row>
-    <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="91"/>
       <c r="B14" s="42"/>
       <c r="C14" s="43"/>
@@ -8907,7 +8889,7 @@
       <c r="L14" s="43"/>
       <c r="M14" s="91"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A15" s="91"/>
       <c r="B15" s="12"/>
       <c r="C15" s="32"/>
@@ -8922,7 +8904,7 @@
       <c r="L15" s="32"/>
       <c r="M15" s="91"/>
     </row>
-    <row r="16" spans="1:13" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" ht="6" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="91"/>
       <c r="B16" s="47"/>
       <c r="C16" s="49"/>
@@ -8937,7 +8919,7 @@
       <c r="L16" s="49"/>
       <c r="M16" s="91"/>
     </row>
-    <row r="17" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="91"/>
       <c r="B17" s="95" t="s">
         <v>41</v>
@@ -8956,7 +8938,7 @@
       <c r="L17" s="32"/>
       <c r="M17" s="91"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A18" s="91"/>
       <c r="B18" s="12"/>
       <c r="C18" s="32"/>
@@ -8971,48 +8953,48 @@
       <c r="L18" s="32"/>
       <c r="M18" s="91"/>
     </row>
-    <row r="19" spans="1:13" s="86" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" s="86" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="94"/>
-      <c r="B19" s="134" t="s">
+      <c r="B19" s="127" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="137" t="s">
+      <c r="C19" s="146" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="137" t="s">
+      <c r="D19" s="146" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="181" t="s">
+      <c r="E19" s="180" t="s">
         <v>45</v>
       </c>
-      <c r="F19" s="181" t="s">
+      <c r="F19" s="180" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="181" t="s">
+      <c r="G19" s="180" t="s">
         <v>38</v>
       </c>
-      <c r="H19" s="137" t="s">
+      <c r="H19" s="146" t="s">
         <v>35</v>
       </c>
-      <c r="I19" s="181" t="s">
+      <c r="I19" s="180" t="s">
         <v>47</v>
       </c>
-      <c r="J19" s="182"/>
-      <c r="K19" s="182"/>
-      <c r="L19" s="137" t="s">
+      <c r="J19" s="181"/>
+      <c r="K19" s="181"/>
+      <c r="L19" s="146" t="s">
         <v>46</v>
       </c>
       <c r="M19" s="94"/>
     </row>
-    <row r="20" spans="1:13" s="86" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" s="86" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="94"/>
-      <c r="B20" s="185"/>
-      <c r="C20" s="185"/>
-      <c r="D20" s="185"/>
-      <c r="E20" s="185"/>
-      <c r="F20" s="185"/>
-      <c r="G20" s="185"/>
-      <c r="H20" s="185"/>
+      <c r="B20" s="179"/>
+      <c r="C20" s="179"/>
+      <c r="D20" s="179"/>
+      <c r="E20" s="179"/>
+      <c r="F20" s="179"/>
+      <c r="G20" s="179"/>
+      <c r="H20" s="179"/>
       <c r="I20" s="85" t="s">
         <v>34</v>
       </c>
@@ -9022,10 +9004,10 @@
       <c r="K20" s="85" t="s">
         <v>36</v>
       </c>
-      <c r="L20" s="185"/>
+      <c r="L20" s="179"/>
       <c r="M20" s="94"/>
     </row>
-    <row r="21" spans="1:13" s="86" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" s="86" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="94"/>
       <c r="B21" s="99"/>
       <c r="C21" s="99"/>
@@ -9040,7 +9022,7 @@
       <c r="L21" s="99"/>
       <c r="M21" s="94"/>
     </row>
-    <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="91"/>
       <c r="B22" s="42"/>
       <c r="C22" s="43"/>
@@ -9064,7 +9046,7 @@
       <c r="L22" s="43"/>
       <c r="M22" s="91"/>
     </row>
-    <row r="23" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="91"/>
       <c r="B23" s="12"/>
       <c r="C23" s="32"/>
@@ -9079,7 +9061,7 @@
       <c r="L23" s="32"/>
       <c r="M23" s="91"/>
     </row>
-    <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="91"/>
       <c r="B24" s="42"/>
       <c r="C24" s="43"/>
@@ -9103,7 +9085,7 @@
       <c r="L24" s="43"/>
       <c r="M24" s="91"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A25" s="91"/>
       <c r="B25" s="12"/>
       <c r="C25" s="32"/>
@@ -9118,7 +9100,7 @@
       <c r="L25" s="32"/>
       <c r="M25" s="91"/>
     </row>
-    <row r="26" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="91"/>
       <c r="B26" s="42"/>
       <c r="C26" s="43"/>
@@ -9142,7 +9124,7 @@
       <c r="L26" s="43"/>
       <c r="M26" s="91"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A27" s="91"/>
       <c r="B27" s="12"/>
       <c r="C27" s="32"/>
@@ -9157,7 +9139,7 @@
       <c r="L27" s="32"/>
       <c r="M27" s="91"/>
     </row>
-    <row r="28" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="91"/>
       <c r="B28" s="42"/>
       <c r="C28" s="43"/>
@@ -9181,7 +9163,7 @@
       <c r="L28" s="43"/>
       <c r="M28" s="91"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A29" s="91"/>
       <c r="B29" s="12"/>
       <c r="C29" s="32"/>
@@ -9196,7 +9178,7 @@
       <c r="L29" s="32"/>
       <c r="M29" s="91"/>
     </row>
-    <row r="30" spans="1:13" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" ht="6" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="91"/>
       <c r="B30" s="47"/>
       <c r="C30" s="49"/>
@@ -9213,6 +9195,16 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="G2:K3"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
     <mergeCell ref="L19:L20"/>
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="I5:K5"/>
@@ -9223,16 +9215,6 @@
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="G19:G20"/>
     <mergeCell ref="H19:H20"/>
-    <mergeCell ref="G2:K3"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>